<commit_message>
fix: update general admissions data
</commit_message>
<xml_diff>
--- a/tables/table_general_100k_rates_2019_2021.xlsx
+++ b/tables/table_general_100k_rates_2019_2021.xlsx
@@ -205,22 +205,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:J16"/>
+      <selection pane="topLeft" activeCell="N22" activeCellId="0" sqref="N22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="8.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="6.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="7.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -239,13 +239,13 @@
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="H1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -257,26 +257,25 @@
         <v>5</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>3637</v>
+        <v>5063</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>3071</v>
+        <v>4393</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>3311</v>
+        <v>4592</v>
       </c>
       <c r="F2" s="3" t="n">
-        <v>-8.96343139950509</v>
-      </c>
-      <c r="G2" s="3"/>
+        <v>-9.30278491013233</v>
+      </c>
+      <c r="G2" s="3" t="n">
+        <v>-4.87067979136637</v>
+      </c>
       <c r="H2" s="3" t="n">
-        <v>-4.72757767395969</v>
+        <v>-4.93187072298826</v>
       </c>
       <c r="I2" s="3" t="n">
-        <v>-4.80013728632364</v>
-      </c>
-      <c r="J2" s="3" t="n">
-        <v>-4.65496275797245</v>
+        <v>-4.80944947398879</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -287,26 +286,25 @@
         <v>6</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>328</v>
+        <v>334</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>421</v>
+        <v>427</v>
       </c>
       <c r="F3" s="3" t="n">
-        <v>48.7632508833922</v>
-      </c>
-      <c r="G3" s="3"/>
+        <v>47.7508650519031</v>
+      </c>
+      <c r="G3" s="3" t="n">
+        <v>21.9952739814482</v>
+      </c>
       <c r="H3" s="3" t="n">
-        <v>22.4770147724043</v>
+        <v>21.7055221702211</v>
       </c>
       <c r="I3" s="3" t="n">
-        <v>22.1835093930172</v>
-      </c>
-      <c r="J3" s="3" t="n">
-        <v>22.7712252011729</v>
+        <v>22.2857156226075</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -317,26 +315,25 @@
         <v>7</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>3355</v>
+        <v>4774</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>2743</v>
+        <v>4059</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>2890</v>
+        <v>4165</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>-13.8599105812221</v>
-      </c>
-      <c r="G4" s="3"/>
+        <v>-12.7565982404692</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>-6.75549480858085</v>
+      </c>
       <c r="H4" s="3" t="n">
-        <v>-7.42587239903673</v>
+        <v>-6.8178799443065</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>-7.50037211790188</v>
-      </c>
-      <c r="J4" s="3" t="n">
-        <v>-7.35131267768034</v>
+        <v>-6.69306790620344</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -347,26 +344,25 @@
         <v>8</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>2191</v>
+        <v>4282</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>1828</v>
+        <v>3774</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>1989</v>
+        <v>3873</v>
       </c>
       <c r="F5" s="3" t="n">
-        <v>-9.21953445915107</v>
-      </c>
-      <c r="G5" s="3"/>
+        <v>-9.55161139654367</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>-4.99770322224804</v>
+      </c>
       <c r="H5" s="3" t="n">
-        <v>-4.89251373929834</v>
+        <v>-5.09897336391733</v>
       </c>
       <c r="I5" s="3" t="n">
-        <v>-5.03535209444925</v>
-      </c>
-      <c r="J5" s="3" t="n">
-        <v>-4.74946053792674</v>
+        <v>-4.89632501387013</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -377,26 +373,25 @@
         <v>9</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>169</v>
+        <v>177</v>
       </c>
       <c r="F6" s="3" t="n">
-        <v>72.4489795918367</v>
-      </c>
-      <c r="G6" s="3"/>
+        <v>66.9811320754717</v>
+      </c>
+      <c r="G6" s="3" t="n">
+        <v>30.8407909322997</v>
+      </c>
       <c r="H6" s="3" t="n">
-        <v>33.2107932663084</v>
+        <v>30.0673198514908</v>
       </c>
       <c r="I6" s="3" t="n">
-        <v>32.3975589887739</v>
-      </c>
-      <c r="J6" s="3" t="n">
-        <v>34.0290227264974</v>
+        <v>31.6188616120973</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -407,26 +402,25 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>2093</v>
+        <v>4177</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>1717</v>
+        <v>3655</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>1821</v>
+        <v>3697</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>-12.9956999522217</v>
-      </c>
-      <c r="G7" s="3"/>
+        <v>-11.4915010773282</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>-6.03780085893659</v>
+      </c>
       <c r="H7" s="3" t="n">
-        <v>-6.99271013306924</v>
+        <v>-6.13971387826559</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>-7.13708317755972</v>
-      </c>
-      <c r="J7" s="3" t="n">
-        <v>-6.8481126332559</v>
+        <v>-5.93577718297168</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -437,26 +431,25 @@
         <v>11</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>4171</v>
+        <v>4296</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>3555</v>
+        <v>3655</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>4000</v>
+        <v>4100</v>
       </c>
       <c r="F8" s="3" t="n">
-        <v>-4.09973627427475</v>
-      </c>
-      <c r="G8" s="3"/>
+        <v>-4.56238361266294</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>-2.33623471196117</v>
+      </c>
       <c r="H8" s="3" t="n">
-        <v>-2.08650743351292</v>
+        <v>-2.77434675912087</v>
       </c>
       <c r="I8" s="3" t="n">
-        <v>-2.53176664676321</v>
-      </c>
-      <c r="J8" s="3" t="n">
-        <v>-1.63921416506163</v>
+        <v>-1.89614847219419</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -467,26 +460,25 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="F9" s="3" t="n">
-        <v>66.7655786350148</v>
-      </c>
-      <c r="G9" s="3"/>
+        <v>65.8823529411765</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>30.0119294325175</v>
+      </c>
       <c r="H9" s="3" t="n">
-        <v>30.287944320593</v>
+        <v>28.2123046139125</v>
       </c>
       <c r="I9" s="3" t="n">
-        <v>28.478929927315</v>
-      </c>
-      <c r="J9" s="3" t="n">
-        <v>32.1224300738594</v>
+        <v>31.8368143031705</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -497,26 +489,25 @@
         <v>13</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>3834</v>
+        <v>3956</v>
       </c>
       <c r="D10" s="2" t="n">
-        <v>3162</v>
+        <v>3260</v>
       </c>
       <c r="E10" s="2" t="n">
-        <v>3439</v>
+        <v>3536</v>
       </c>
       <c r="F10" s="3" t="n">
-        <v>-10.302556077204</v>
-      </c>
-      <c r="G10" s="3"/>
+        <v>-10.6167846309403</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <v>-5.62582718839986</v>
+      </c>
       <c r="H10" s="3" t="n">
-        <v>-5.45881971713331</v>
+        <v>-6.07423848823994</v>
       </c>
       <c r="I10" s="3" t="n">
-        <v>-5.91477914966812</v>
-      </c>
-      <c r="J10" s="3" t="n">
-        <v>-5.00065059637928</v>
+        <v>-5.17527512663688</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -527,26 +518,25 @@
         <v>14</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>6482</v>
+        <v>6566</v>
       </c>
       <c r="D11" s="2" t="n">
-        <v>5520</v>
+        <v>5588</v>
       </c>
       <c r="E11" s="2" t="n">
-        <v>5913</v>
+        <v>5981</v>
       </c>
       <c r="F11" s="3" t="n">
-        <v>-8.77815489046591</v>
-      </c>
-      <c r="G11" s="3"/>
+        <v>-8.90953396283887</v>
+      </c>
+      <c r="G11" s="3" t="n">
+        <v>-4.60750298742759</v>
+      </c>
       <c r="H11" s="3" t="n">
-        <v>-4.53472053520966</v>
+        <v>-5.11507427248935</v>
       </c>
       <c r="I11" s="3" t="n">
-        <v>-5.0457782114764</v>
-      </c>
-      <c r="J11" s="3" t="n">
-        <v>-4.02091227088529</v>
+        <v>-4.09721653336038</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -557,26 +547,25 @@
         <v>15</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>786</v>
+        <v>789</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>954</v>
+        <v>956</v>
       </c>
       <c r="F12" s="3" t="n">
-        <v>40.2941176470588</v>
-      </c>
-      <c r="G12" s="3"/>
+        <v>39.9707174231332</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <v>18.5625923761527</v>
+      </c>
       <c r="H12" s="3" t="n">
-        <v>18.6594271269781</v>
+        <v>16.83257341946</v>
       </c>
       <c r="I12" s="3" t="n">
-        <v>16.9251642120325</v>
-      </c>
-      <c r="J12" s="3" t="n">
-        <v>20.4194130578239</v>
+        <v>20.3182288939667</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -587,26 +576,25 @@
         <v>16</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>5803</v>
+        <v>5884</v>
       </c>
       <c r="D13" s="2" t="n">
-        <v>4734</v>
+        <v>4800</v>
       </c>
       <c r="E13" s="2" t="n">
-        <v>4960</v>
+        <v>5025</v>
       </c>
       <c r="F13" s="3" t="n">
-        <v>-14.5269688092366</v>
-      </c>
-      <c r="G13" s="3"/>
+        <v>-14.5989123045547</v>
+      </c>
+      <c r="G13" s="3" t="n">
+        <v>-7.7577701373949</v>
+      </c>
       <c r="H13" s="3" t="n">
-        <v>-7.72059202991111</v>
+        <v>-8.28548949059822</v>
       </c>
       <c r="I13" s="3" t="n">
-        <v>-8.25211774518345</v>
-      </c>
-      <c r="J13" s="3" t="n">
-        <v>-7.18598701101833</v>
+        <v>-7.22701432121317</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -617,26 +605,25 @@
         <v>17</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>11023</v>
+        <v>11086</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>9360</v>
+        <v>9409</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>9669</v>
+        <v>9718</v>
       </c>
       <c r="F14" s="3" t="n">
-        <v>-12.2834074208473</v>
-      </c>
-      <c r="G14" s="3"/>
+        <v>-12.3398881472127</v>
+      </c>
+      <c r="G14" s="3" t="n">
+        <v>-6.44527338846238</v>
+      </c>
       <c r="H14" s="3" t="n">
-        <v>-6.41681368813354</v>
+        <v>-6.93078705917676</v>
       </c>
       <c r="I14" s="3" t="n">
-        <v>-6.90376385044337</v>
-      </c>
-      <c r="J14" s="3" t="n">
-        <v>-5.92731647912901</v>
+        <v>-5.95722694115087</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -647,26 +634,25 @@
         <v>18</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>1212</v>
+        <v>1214</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>1422</v>
+        <v>1424</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>1572</v>
+        <v>1574</v>
       </c>
       <c r="F15" s="3" t="n">
-        <v>29.7029702970297</v>
-      </c>
-      <c r="G15" s="3"/>
+        <v>29.6540362438221</v>
+      </c>
+      <c r="G15" s="3" t="n">
+        <v>13.6684857799816</v>
+      </c>
       <c r="H15" s="3" t="n">
-        <v>13.706858530392</v>
+        <v>12.0885859787854</v>
       </c>
       <c r="I15" s="3" t="n">
-        <v>12.1253012497393</v>
-      </c>
-      <c r="J15" s="3" t="n">
-        <v>15.3107240983279</v>
+        <v>15.2706544264846</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -677,26 +663,25 @@
         <v>19</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>9811</v>
+        <v>9872</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>7939</v>
+        <v>7986</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>8097</v>
+        <v>8144</v>
       </c>
       <c r="F16" s="3" t="n">
-        <v>-17.4701865253287</v>
-      </c>
-      <c r="G16" s="3"/>
+        <v>-17.5040518638574</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <v>-9.35840909194882</v>
+      </c>
       <c r="H16" s="3" t="n">
-        <v>-9.34443371654697</v>
+        <v>-9.86591180217631</v>
       </c>
       <c r="I16" s="3" t="n">
-        <v>-9.8535246707375</v>
-      </c>
-      <c r="J16" s="3" t="n">
-        <v>-8.83246773481163</v>
+        <v>-8.84804887235902</v>
       </c>
     </row>
   </sheetData>

</xml_diff>